<commit_message>
add new software list
</commit_message>
<xml_diff>
--- a/StateOfPractice/DomainMeasurements/InverseKinematics-Ryan/Software_List.xlsx
+++ b/StateOfPractice/DomainMeasurements/InverseKinematics-Ryan/Software_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\course\ResearchProject\AIMSS\StateOfPractice\DomainMeasurements\InverseKinematics-Ryan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805D9439-9B4A-4EDF-9C1D-824508253714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8AEB01-9BD3-4257-863A-1A03D8E440C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{2279FB42-8099-4FD6-9EF2-F606B56203F5}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2279FB42-8099-4FD6-9EF2-F606B56203F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,253 +34,341 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>Software / Library</t>
   </si>
   <si>
+    <t>Widely used numerical IK/Jacobian solver in ROS and industry; mature implementation, serves as a baseline reference.</t>
+  </si>
+  <si>
+    <t>TRAC-IK</t>
+  </si>
+  <si>
+    <t>Faster and more reliable than KDL in ROS contexts, higher success rates, commonly used as a drop-in replacement.</t>
+  </si>
+  <si>
+    <t>Analytical IK “compiler” that generates highly optimized C++ solvers for specific arms; widely adopted in MoveIt.</t>
+  </si>
+  <si>
+    <t>Analytical IK for 6-DOF offset wrist manipulators, very fast and supports many industrial arms.</t>
+  </si>
+  <si>
+    <t>MoveIt/MoveIt2 plugin from PickNik; supports multiple constraints, weight configuration, and offers good performance and usability.</t>
+  </si>
+  <si>
+    <t>Levenberg–Marquardt numerical IK plugin, the traditional baseline solver in MoveIt.</t>
+  </si>
+  <si>
+    <t>Kinematics interface of the Tesseract ecosystem, integrates multiple solvers (KDL, OPW, etc.) in a production-ready framework.</t>
+  </si>
+  <si>
+    <t>Optimization-based multi-objective IK solver (MoveIt plugin), well-suited for complex constraint scenarios.</t>
+  </si>
+  <si>
+    <t>Null-Space Saturation (SNS) IK solver; supports prioritized tasks and joint limit handling.</t>
+  </si>
+  <si>
+    <t>Constraint-based, set-based task-space IK framework supporting multiple task priorities and closed-loop control.</t>
+  </si>
+  <si>
+    <t>Differential IK library built on Pinocchio; well-suited for multi-chain and humanoid robots.</t>
+  </si>
+  <si>
+    <t>Differential IK solver with joint/velocity limits and collision avoidance, supporting closed-loop constraints.</t>
+  </si>
+  <si>
+    <t>Formulates IK as a quadratic program for real-time solutions; robust to redundancy and collision avoidance.</t>
+  </si>
+  <si>
+    <t>Graph-based and distance-geometry approach to IK, offering an alternative to traditional numerical solvers.</t>
+  </si>
+  <si>
+    <t>Generative graph-model-based learning IK framework, enabling cross-robot generalization.</t>
+  </si>
+  <si>
+    <t>Uses normalizing flows to learn the distribution of IK solutions, capable of handling multiple solutions and generalizing to unseen poses.</t>
+  </si>
+  <si>
+    <t>IKBT (Behavior Tree)</t>
+  </si>
+  <si>
+    <t>Organizes symbolic/analytic IK solving steps into behavior trees, allowing composable reasoning pipelines.</t>
+  </si>
+  <si>
+    <t>IKPy</t>
+  </si>
+  <si>
+    <t>tinyik</t>
+  </si>
+  <si>
+    <t>Minimal Python IK solver, useful for teaching and quick prototyping of small-scale systems.</t>
+  </si>
+  <si>
+    <t>rpiRobotics/ik-geo</t>
+  </si>
+  <si>
+    <t>Educational geometric IK implementation; good reference for understanding analytic geometry methods.</t>
+  </si>
+  <si>
+    <t>Analytical and redundancy-resolution solver for 7-DOF KUKA iiwa, representing 7-DOF arms.</t>
+  </si>
+  <si>
+    <t>Analytical IK solver for NAO humanoid robot, with well-documented implementation and publications.</t>
+  </si>
+  <si>
+    <t>Python implementation of kinematics (including IK) for UR series manipulators.</t>
+  </si>
+  <si>
+    <t>IK solver for Delta parallel robots, covering the parallel manipulator family.</t>
+  </si>
+  <si>
+    <t>IK implementation for Stewart platforms, representing 6-DOF parallel mechanisms.</t>
+  </si>
+  <si>
+    <t>Rigid Body Dynamics Library, includes damped least-squares iterative IK API; widely used as a dynamics base.</t>
+  </si>
+  <si>
+    <t>A fork/extension of RBDL providing similar IK interfaces; useful for comparison and validation.</t>
+  </si>
+  <si>
+    <t>Orocos KDL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Close source, can not get soruce code, but widely use </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://moveit.picknik.ai/main/doc/how_to_guides/trac_ik/trac_ik_tutorial.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/orocos/orocos_kinematics_dynamics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IKFast (OpenRAVE / MoveIt)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://moveit.picknik.ai/main/doc/examples/ikfast/ikfast_tutorial.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OPW Kinematics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/Jmeyer1292/opw_kinematics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pick-IK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://moveit.picknik.ai/main/doc/how_to_guides/pick_ik/pick_ik_tutorial.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LMA Kinematics Plugin (MoveIt)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://moveit.picknik.ai/humble/doc/examples/kinematics_configuration/kinematics_configuration_tutorial.html#the-lma-kinematics-plugin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tesseract Kinematics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/tesseract-robotics/tesseract</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bio_ik</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/TAMS-Group/bio_ik</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RethinkRobotics sns_ik</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/RethinkRobotics-opensource/sns_ik</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CASCLIK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/mahaarbo/casclik</t>
+  </si>
+  <si>
+    <t>pink (Pinocchio-based IK)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mink (MuJoCo-based IK)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/stephane-caron/pink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/kevinzakka/mink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QP_IK_solver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/SinaMirrazavi/QP_IK_solver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GraphIK (UTIAS-STARS)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/utiasSTARS/GraphIK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/utiasSTARS/generative-graphik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generative-graphik </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IKFlow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/uw-biorobotics/IKBT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/jstmn/ikflow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>General-purpose Python IK library; supports URDF/DH input and multiple joint types; widely used in education and prototyping.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/Phylliade/ikpy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/lanius/tinyik</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/rpiRobotics/ik-geo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>neuebot/kuka_iiwa_ik</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/neuebot/kuka_iiwa_ik</t>
+  </si>
+  <si>
+    <t>NAOKinematics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/kouretes/NAOKinematics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mc-capolei/python-Universal-robot-kinematics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/mc-capolei/python-Universal-robot-kinematics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tinkersprojects/Delta-Kinematics-Library</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/tinkersprojects/Delta-Kinematics-Library</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hbartle/Stewart_Platform</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/hbartle/Stewart_Platform</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RBDL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/rbdl/rbdl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RobotDynamicsLibrary (EricVoll)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/EricVoll/RobotDynamicsLibrary</t>
+  </si>
+  <si>
+    <t>Drake IK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/RobotLocomotion/drake?tab=readme-ov-file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pinocchio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/stack-of-tasks/pinocchio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Reason for Inclusion</t>
-  </si>
-  <si>
-    <t>Widely used numerical IK/Jacobian solver in ROS and industry; mature implementation, serves as a baseline reference.</t>
-  </si>
-  <si>
-    <t>TRAC-IK</t>
-  </si>
-  <si>
-    <t>Faster and more reliable than KDL in ROS contexts, higher success rates, commonly used as a drop-in replacement.</t>
-  </si>
-  <si>
-    <t>Analytical IK “compiler” that generates highly optimized C++ solvers for specific arms; widely adopted in MoveIt.</t>
-  </si>
-  <si>
-    <t>Analytical IK for 6-DOF offset wrist manipulators, very fast and supports many industrial arms.</t>
-  </si>
-  <si>
-    <t>MoveIt/MoveIt2 plugin from PickNik; supports multiple constraints, weight configuration, and offers good performance and usability.</t>
-  </si>
-  <si>
-    <t>Levenberg–Marquardt numerical IK plugin, the traditional baseline solver in MoveIt.</t>
-  </si>
-  <si>
-    <t>Tesseract Kinematics</t>
-  </si>
-  <si>
-    <t>Kinematics interface of the Tesseract ecosystem, integrates multiple solvers (KDL, OPW, etc.) in a production-ready framework.</t>
-  </si>
-  <si>
-    <t>bio_ik</t>
-  </si>
-  <si>
-    <t>Optimization-based multi-objective IK solver (MoveIt plugin), well-suited for complex constraint scenarios.</t>
-  </si>
-  <si>
-    <t>RethinkRobotics sns_ik</t>
-  </si>
-  <si>
-    <t>Null-Space Saturation (SNS) IK solver; supports prioritized tasks and joint limit handling.</t>
-  </si>
-  <si>
-    <t>moveit_whole_body_ik</t>
-  </si>
-  <si>
-    <t>Whole-body and multi-chain IK prototype plugin, good for studying coordinated motion of complex systems.</t>
-  </si>
-  <si>
-    <t>CASCLIK</t>
-  </si>
-  <si>
-    <t>Constraint-based, set-based task-space IK framework supporting multiple task priorities and closed-loop control.</t>
-  </si>
-  <si>
-    <t>pink (Pinocchio-based IK)</t>
-  </si>
-  <si>
-    <t>Differential IK library built on Pinocchio; well-suited for multi-chain and humanoid robots.</t>
-  </si>
-  <si>
-    <t>mink (MuJoCo-based IK)</t>
-  </si>
-  <si>
-    <t>Differential IK solver with joint/velocity limits and collision avoidance, supporting closed-loop constraints.</t>
-  </si>
-  <si>
-    <t>QP_IK_solver (Mirrazavi et al.)</t>
-  </si>
-  <si>
-    <t>Formulates IK as a quadratic program for real-time solutions; robust to redundancy and collision avoidance.</t>
-  </si>
-  <si>
-    <t>mrsp/whole_body_ik</t>
-  </si>
-  <si>
-    <t>Research-oriented whole-body IK solver with configurable task priorities and weights.</t>
-  </si>
-  <si>
-    <t>GraphIK (UTIAS-STARS)</t>
-  </si>
-  <si>
-    <t>Graph-based and distance-geometry approach to IK, offering an alternative to traditional numerical solvers.</t>
-  </si>
-  <si>
-    <t>generative-graphik (UTIAS-STARS)</t>
-  </si>
-  <si>
-    <t>Generative graph-model-based learning IK framework, enabling cross-robot generalization.</t>
-  </si>
-  <si>
-    <t>IKFlow</t>
-  </si>
-  <si>
-    <t>Uses normalizing flows to learn the distribution of IK solutions, capable of handling multiple solutions and generalizing to unseen poses.</t>
-  </si>
-  <si>
-    <t>IKBT (Behavior Tree)</t>
-  </si>
-  <si>
-    <t>Organizes symbolic/analytic IK solving steps into behavior trees, allowing composable reasoning pipelines.</t>
-  </si>
-  <si>
-    <t>IKPy</t>
-  </si>
-  <si>
-    <t>General-purpose Python IK library; supports URDF/DH input and multiple joint types; widely used in education and prototyping.</t>
-  </si>
-  <si>
-    <t>tinyik</t>
-  </si>
-  <si>
-    <t>Minimal Python IK solver, useful for teaching and quick prototyping of small-scale systems.</t>
-  </si>
-  <si>
-    <t>rpiRobotics/ik-geo</t>
-  </si>
-  <si>
-    <t>Educational geometric IK implementation; good reference for understanding analytic geometry methods.</t>
-  </si>
-  <si>
-    <t>neuebot/kuka_iiwa_ik</t>
-  </si>
-  <si>
-    <t>Analytical and redundancy-resolution solver for 7-DOF KUKA iiwa, representing 7-DOF arms.</t>
-  </si>
-  <si>
-    <t>NAOKinematics</t>
-  </si>
-  <si>
-    <t>Analytical IK solver for NAO humanoid robot, with well-documented implementation and publications.</t>
-  </si>
-  <si>
-    <t>mc-capolei/python-Universal-robot-kinematics</t>
-  </si>
-  <si>
-    <t>Python implementation of kinematics (including IK) for UR series manipulators.</t>
-  </si>
-  <si>
-    <t>OPW Kinematics (duplicate entry for mechanism coverage)</t>
-  </si>
-  <si>
-    <t>Included to explicitly represent the common 6R industrial arm family with offset wrist.</t>
-  </si>
-  <si>
-    <t>tinkersprojects/Delta-Kinematics-Library</t>
-  </si>
-  <si>
-    <t>IK solver for Delta parallel robots, covering the parallel manipulator family.</t>
-  </si>
-  <si>
-    <t>hbartle/Stewart_Platform</t>
-  </si>
-  <si>
-    <t>IK implementation for Stewart platforms, representing 6-DOF parallel mechanisms.</t>
-  </si>
-  <si>
-    <t>RBDL</t>
-  </si>
-  <si>
-    <t>Rigid Body Dynamics Library, includes damped least-squares iterative IK API; widely used as a dynamics base.</t>
-  </si>
-  <si>
-    <t>RobotDynamicsLibrary (EricVoll)</t>
-  </si>
-  <si>
-    <t>A fork/extension of RBDL providing similar IK interfaces; useful for comparison and validation.</t>
-  </si>
-  <si>
-    <t>Orocos KDL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Close source, can not get soruce code, but widely use </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pending</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)MATLAB &amp; Simulink Robotics System Toolbox</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://moveit.picknik.ai/main/doc/how_to_guides/trac_ik/trac_ik_tutorial.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://github.com/orocos/orocos_kinematics_dynamics</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IKFast (OpenRAVE / MoveIt)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://moveit.picknik.ai/main/doc/examples/ikfast/ikfast_tutorial.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OPW Kinematics</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://github.com/Jmeyer1292/opw_kinematics</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pick-IK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://moveit.picknik.ai/main/doc/how_to_guides/pick_ik/pick_ik_tutorial.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LMA Kinematics Plugin (MoveIt)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://moveit.picknik.ai/humble/doc/examples/kinematics_configuration/kinematics_configuration_tutorial.html#the-lma-kinematics-plugin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Part of MIT’s Drake robotics toolbox; provides a well-maintained, optimization-based IK solver supporting position/orientation constraints, joint limits, and redundancy resolution. Widely used in academia and industry, making it a strong representative of state-of-the-art optimization IK.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>High-performance rigid-body dynamics library developed by INRIA; includes fast Jacobian and differential IK computation. Frequently used in legged robotics and humanoid research, with excellent documentation and active community support.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.mathworks.com/products/robotics.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MATLAB &amp; Simulink Robotics System Toolbox</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -288,7 +376,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +410,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -348,7 +444,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -360,6 +456,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -676,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354D475D-67CE-47C1-879A-864A87C4D259}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -689,12 +791,15 @@
     <col min="4" max="4" width="89.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>87</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
@@ -702,13 +807,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
@@ -716,13 +821,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
@@ -730,13 +835,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
@@ -744,13 +849,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
@@ -758,13 +863,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
@@ -772,288 +877,349 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="228" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="171" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>15</v>
+      <c r="B11" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="213.75" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="142.5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="199.5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="185.25" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="156.75" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>25</v>
+      <c r="B16" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="199.5" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="185.25" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="242.25" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="171" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="228" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="156.75" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="199.5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="171" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="171" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="D24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="142.5" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="171" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="128.25" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="142.5" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="199.5" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="156.75" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="D30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>58</v>
+        <v>33</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1064,6 +1230,26 @@
     <hyperlink ref="D5" r:id="rId3" xr:uid="{46257C39-5BD0-4E0F-82DE-F51185D7AC5E}"/>
     <hyperlink ref="D6" r:id="rId4" xr:uid="{A5D6C053-25C2-4D69-8E16-64542131C8FF}"/>
     <hyperlink ref="D7" r:id="rId5" location="the-lma-kinematics-plugin" xr:uid="{64C6DC26-5389-4561-806B-09D910B907E6}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{877A4161-2F74-4120-8458-007B869F6808}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{EB208228-53E8-4BEC-B279-DCFD2E3D7FEE}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{09DA4EF2-973B-4CEE-92A6-C07E44F61A9A}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{8558024D-AB6E-4E22-8BA0-9A54E2E44AA9}"/>
+    <hyperlink ref="D13" r:id="rId10" xr:uid="{AA5FFC52-577C-4E4B-8249-CB28513BAD1F}"/>
+    <hyperlink ref="D14" r:id="rId11" xr:uid="{B477B5E8-3A6A-4E1A-9B0C-CACC9E0FEBF2}"/>
+    <hyperlink ref="D15" r:id="rId12" xr:uid="{0DBF26C7-B4F7-4A38-8B49-E53C2EF4113D}"/>
+    <hyperlink ref="D16" r:id="rId13" xr:uid="{A9946ABD-5633-4DD6-B240-7EF0E88EAC39}"/>
+    <hyperlink ref="D17" r:id="rId14" xr:uid="{60736914-D561-4CE5-88AB-3D541B997633}"/>
+    <hyperlink ref="D19" r:id="rId15" xr:uid="{FC9128E5-AE14-4A26-9E20-C0B418C115E6}"/>
+    <hyperlink ref="D20" r:id="rId16" xr:uid="{5628DB8F-F9F4-4AE8-9C2A-2F69359936A5}"/>
+    <hyperlink ref="D21" r:id="rId17" xr:uid="{5E1E8C0E-C436-4478-AF98-A307EC56499A}"/>
+    <hyperlink ref="D22" r:id="rId18" xr:uid="{D2ED9F77-6F13-4505-BB93-C8D02BF77E0D}"/>
+    <hyperlink ref="D23" r:id="rId19" xr:uid="{EF32EB37-AD6B-42A7-968A-16EB7847ADB4}"/>
+    <hyperlink ref="D25" r:id="rId20" xr:uid="{334A8B43-0B47-42F8-B0BC-1F923B2C111C}"/>
+    <hyperlink ref="D26" r:id="rId21" xr:uid="{47BFFC86-DEA4-4994-858F-668A807D0B97}"/>
+    <hyperlink ref="D27" r:id="rId22" xr:uid="{BD658A75-9E84-41EA-AE5A-055FC061E387}"/>
+    <hyperlink ref="D28" r:id="rId23" xr:uid="{D02458EE-4797-42CD-9F33-007C9109496E}"/>
+    <hyperlink ref="D29" r:id="rId24" xr:uid="{01D23E18-CA30-477D-8CC0-5A45DE398E76}"/>
+    <hyperlink ref="D31" r:id="rId25" xr:uid="{18AEEAF3-98E0-4149-9273-520756D58AA6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>